<commit_message>
flexen met mn punten
</commit_message>
<xml_diff>
--- a/resultaten.xlsx
+++ b/resultaten.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikki\Documents\School\2020-2021\MOA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikki\Documents\School\2020-2021\MOA\2021_MOA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FAE6DC9E-B757-4B71-9A5B-A95E71435FFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F469ACFA-0036-4B35-9840-A6C365D79D67}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{AA9A4842-A447-4D22-9AB9-6BB7FD62ABEA}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>opdracht</t>
   </si>
@@ -83,9 +82,6 @@
   </si>
   <si>
     <t>totaal</t>
-  </si>
-  <si>
-    <t>afwachten</t>
   </si>
   <si>
     <t>mee bezig</t>
@@ -274,7 +270,77 @@
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -648,7 +714,7 @@
   <dimension ref="B1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -695,8 +761,8 @@
       <c r="D5" s="8">
         <v>5</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>16</v>
+      <c r="E5" s="13">
+        <v>5</v>
       </c>
       <c r="F5" s="9"/>
     </row>
@@ -776,7 +842,7 @@
       </c>
       <c r="F11" s="9"/>
       <c r="H11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I11">
         <f>D18*0.8</f>
@@ -804,7 +870,9 @@
       <c r="D13" s="8">
         <v>10</v>
       </c>
-      <c r="E13" s="13"/>
+      <c r="E13" s="13" t="s">
+        <v>16</v>
+      </c>
       <c r="F13" s="9"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
@@ -839,8 +907,8 @@
       <c r="D16" s="11">
         <v>10</v>
       </c>
-      <c r="E16" s="14" t="s">
-        <v>17</v>
+      <c r="E16" s="14">
+        <v>10</v>
       </c>
       <c r="F16" s="9"/>
     </row>
@@ -862,7 +930,7 @@
       </c>
       <c r="E18" s="3">
         <f>SUM(E5:E16)</f>
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="F18" s="9"/>
     </row>
@@ -882,28 +950,33 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E5:E15">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D16">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="between">
       <formula>7</formula>
       <formula>14</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="lessThan">
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:E16">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="afwachten">
+    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="afwachten">
       <formula>NOT(ISERROR(SEARCH("afwachten",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="mee bezig">
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="mee bezig">
       <formula>NOT(ISERROR(SEARCH("mee bezig",E5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -911,21 +984,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C84017735238684C892F000A02E68156" ma:contentTypeVersion="9" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="ed9dda1fbe5757936e109436b33f26ff">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8bb13e81-87ff-48a1-b595-5e203e61adfb" xmlns:ns4="98ffe9ea-2d43-44e2-a350-2abbaa7b30b6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="59dfc4e2e9f9e362dd5effae700ea012" ns3:_="" ns4:_="">
     <xsd:import namespace="8bb13e81-87ff-48a1-b595-5e203e61adfb"/>
@@ -1120,32 +1178,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C21B28B7-C6B3-4446-A109-8B00375F7012}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8bb13e81-87ff-48a1-b595-5e203e61adfb"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="98ffe9ea-2d43-44e2-a350-2abbaa7b30b6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EF62A16-162E-44F5-8E92-94F4F8650018}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6AE567A-0858-407C-81BA-5637E2F24CDA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1162,4 +1210,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EF62A16-162E-44F5-8E92-94F4F8650018}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C21B28B7-C6B3-4446-A109-8B00375F7012}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8bb13e81-87ff-48a1-b595-5e203e61adfb"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="98ffe9ea-2d43-44e2-a350-2abbaa7b30b6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>